<commit_message>
Updated to point at mapserver instead of fs
</commit_message>
<xml_diff>
--- a/Census_Data_Downloads/water_info.xlsx
+++ b/Census_Data_Downloads/water_info.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcclary\Documents\GitHub\Demographics\Census_Data_Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0B5F23-876D-47D2-82C9-8114E901258A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F9A5D2-66BF-4210-A0F1-4205F0E88318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D881382-661F-4226-8308-3F4C037D2227}"/>
+    <workbookView xWindow="28680" yWindow="525" windowWidth="29040" windowHeight="15720" xr2:uid="{1D881382-661F-4226-8308-3F4C037D2227}"/>
   </bookViews>
   <sheets>
-    <sheet name="water_use" sheetId="1" r:id="rId1"/>
+    <sheet name="water_use_statistics" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -254,13 +254,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -579,7 +579,7 @@
   <dimension ref="A1:D294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Enrollment, Water Use and SH visitors
</commit_message>
<xml_diff>
--- a/Census_Data_Downloads/water_info.xlsx
+++ b/Census_Data_Downloads/water_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcclary\Documents\GitHub\Demographics\Census_Data_Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F9A5D2-66BF-4210-A0F1-4205F0E88318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AEA2FA-F7EC-4AF8-A41C-B1923B6C462B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="525" windowWidth="29040" windowHeight="15720" xr2:uid="{1D881382-661F-4226-8308-3F4C037D2227}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D881382-661F-4226-8308-3F4C037D2227}"/>
   </bookViews>
   <sheets>
     <sheet name="water_use_statistics" sheetId="1" r:id="rId1"/>
@@ -579,7 +579,7 @@
   <dimension ref="A1:D294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>